<commit_message>
modifier les fichier R de génération bilan pour qu'ils travaillent avec contrat_notes.R et MCC_24-25.R dans main
</commit_message>
<xml_diff>
--- a/Fichiers/Bilans/bilanContrats.xlsx
+++ b/Fichiers/Bilans/bilanContrats.xlsx
@@ -23,100 +23,100 @@
     <t xml:space="preserve">Code.EC</t>
   </si>
   <si>
-    <t xml:space="preserve">Garnier_Camille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dubois_Zoé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laurent_Zoé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fontaine_Chloé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richard_Léo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David_Arthur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roger_Jules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michel_Alice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leroy_Louise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David_Louis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fournier_Camille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dubois_Lucas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas_Noah_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garnier_Manon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bertrand_Noah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garcia_Louise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morin_Zoé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laurent_Camille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roger_Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roux_Gabriel_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chevalier_Lucas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David_Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petit_Adam_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bertrand_Hugo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moulin_Zoé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bertrand_Chloé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durand_Alice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durand_Jules_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leroy_Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petit_Jules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petit_Louise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fontaine_Manon</t>
+    <t xml:space="preserve">Roger_Lina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David_Camille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garcia_Léo_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertrand_Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chevalier_Jade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dubois_Emma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vincent_Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durand_Camille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morin_Arthur_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert_Raphaël</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert_Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas_Noah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David_Zoé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moulin_Chloé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fontaine_Léo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger_Louise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger_Sarah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laurent_Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard_Jade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger_Lucas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michel_Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leroy_Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin_Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernard_Raphaël</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David_Léo_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michel_Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durand_Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moulin_Hugo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leroy_Emma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petit_Gabriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertrand_Emma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petit_Noah</t>
   </si>
   <si>
     <t xml:space="preserve">Sciences expérimentales (UE-STP03-SE)</t>
@@ -128,10 +128,10 @@
     <t xml:space="preserve">EC-STP03-ACSA</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">Chimie 3</t>
@@ -806,7 +806,7 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
@@ -815,10 +815,10 @@
         <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>38</v>
@@ -833,22 +833,22 @@
         <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s">
         <v>38</v>
@@ -857,43 +857,43 @@
         <v>39</v>
       </c>
       <c r="V2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE2" t="s">
         <v>38</v>
       </c>
       <c r="AF2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG2" t="s">
         <v>39</v>
       </c>
       <c r="AH2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI2" t="s">
         <v>39</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
@@ -910,7 +910,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -919,34 +919,34 @@
         <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
         <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
         <v>39</v>
@@ -955,7 +955,7 @@
         <v>38</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s">
         <v>38</v>
@@ -964,51 +964,51 @@
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -1029,10 +1029,10 @@
         <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
         <v>39</v>
@@ -1047,75 +1047,75 @@
         <v>39</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q4" t="s">
         <v>39</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S4" t="s">
         <v>38</v>
       </c>
       <c r="T4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE4" t="s">
         <v>39</v>
       </c>
       <c r="AF4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG4" t="s">
         <v>39</v>
       </c>
       <c r="AH4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -1124,7 +1124,7 @@
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
@@ -1139,7 +1139,7 @@
         <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
         <v>39</v>
@@ -1151,22 +1151,22 @@
         <v>38</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q5" t="s">
         <v>39</v>
       </c>
       <c r="R5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S5" t="s">
         <v>39</v>
@@ -1178,34 +1178,34 @@
         <v>39</v>
       </c>
       <c r="V5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF5" t="s">
         <v>38</v>
@@ -1214,7 +1214,7 @@
         <v>39</v>
       </c>
       <c r="AH5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI5" t="s">
         <v>39</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
@@ -1231,13 +1231,13 @@
         <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
@@ -1246,85 +1246,85 @@
         <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R6" t="s">
         <v>38</v>
       </c>
       <c r="S6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
       </c>
       <c r="U6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF6" t="s">
         <v>39</v>
       </c>
       <c r="AG6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
@@ -1338,16 +1338,16 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
         <v>39</v>
@@ -1362,58 +1362,58 @@
         <v>38</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" t="s">
         <v>39</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U7" t="s">
         <v>38</v>
       </c>
       <c r="V7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD7" t="s">
         <v>38</v>
@@ -1422,21 +1422,21 @@
         <v>38</v>
       </c>
       <c r="AF7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -1445,31 +1445,31 @@
         <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
         <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M8" t="s">
         <v>39</v>
@@ -1478,55 +1478,55 @@
         <v>39</v>
       </c>
       <c r="O8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P8" t="s">
         <v>38</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U8" t="s">
         <v>38</v>
       </c>
       <c r="V8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y8" t="s">
         <v>38</v>
       </c>
       <c r="Z8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB8" t="s">
         <v>38</v>
       </c>
       <c r="AC8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD8" t="s">
         <v>38</v>
       </c>
       <c r="AE8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF8" t="s">
         <v>39</v>
@@ -1535,7 +1535,7 @@
         <v>38</v>
       </c>
       <c r="AH8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI8" t="s">
         <v>39</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
@@ -1552,16 +1552,16 @@
         <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
@@ -1576,49 +1576,49 @@
         <v>38</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N9" t="s">
         <v>39</v>
       </c>
       <c r="O9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q9" t="s">
         <v>38</v>
       </c>
       <c r="R9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U9" t="s">
         <v>38</v>
       </c>
       <c r="V9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W9" t="s">
         <v>38</v>
       </c>
       <c r="X9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y9" t="s">
         <v>38</v>
       </c>
       <c r="Z9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA9" t="s">
         <v>38</v>
@@ -1627,10 +1627,10 @@
         <v>38</v>
       </c>
       <c r="AC9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE9" t="s">
         <v>38</v>
@@ -1642,7 +1642,7 @@
         <v>38</v>
       </c>
       <c r="AH9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI9" t="s">
         <v>39</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
@@ -1662,19 +1662,19 @@
         <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
         <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
         <v>39</v>
@@ -1683,16 +1683,16 @@
         <v>38</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M10" t="s">
         <v>39</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P10" t="s">
         <v>39</v>
@@ -1701,40 +1701,40 @@
         <v>39</v>
       </c>
       <c r="R10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W10" t="s">
         <v>39</v>
       </c>
       <c r="X10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB10" t="s">
         <v>38</v>
       </c>
       <c r="AC10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD10" t="s">
         <v>38</v>
@@ -1743,13 +1743,13 @@
         <v>38</v>
       </c>
       <c r="AF10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG10" t="s">
         <v>39</v>
       </c>
       <c r="AH10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI10" t="s">
         <v>39</v>
@@ -1766,16 +1766,16 @@
         <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
         <v>39</v>
@@ -1802,16 +1802,16 @@
         <v>39</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" t="s">
         <v>39</v>
       </c>
       <c r="R11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T11" t="s">
         <v>39</v>
@@ -1820,10 +1820,10 @@
         <v>39</v>
       </c>
       <c r="V11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X11" t="s">
         <v>39</v>
@@ -1835,28 +1835,28 @@
         <v>39</v>
       </c>
       <c r="AA11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB11" t="s">
         <v>38</v>
       </c>
       <c r="AC11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD11" t="s">
         <v>38</v>
       </c>
       <c r="AE11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI11" t="s">
         <v>38</v>
@@ -1876,13 +1876,13 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
         <v>39</v>
@@ -1894,13 +1894,13 @@
         <v>38</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N12" t="s">
         <v>38</v>
@@ -1912,19 +1912,19 @@
         <v>39</v>
       </c>
       <c r="Q12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R12" t="s">
         <v>39</v>
       </c>
       <c r="S12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V12" t="s">
         <v>39</v>
@@ -1933,7 +1933,7 @@
         <v>38</v>
       </c>
       <c r="X12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y12" t="s">
         <v>38</v>
@@ -1945,13 +1945,13 @@
         <v>38</v>
       </c>
       <c r="AB12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC12" t="s">
         <v>39</v>
       </c>
       <c r="AD12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE12" t="s">
         <v>38</v>
@@ -1960,7 +1960,7 @@
         <v>39</v>
       </c>
       <c r="AG12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH12" t="s">
         <v>39</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>63</v>
@@ -1983,13 +1983,13 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
         <v>39</v>
@@ -2001,13 +2001,13 @@
         <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N13" t="s">
         <v>38</v>
@@ -2019,19 +2019,19 @@
         <v>39</v>
       </c>
       <c r="Q13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R13" t="s">
         <v>39</v>
       </c>
       <c r="S13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V13" t="s">
         <v>39</v>
@@ -2040,7 +2040,7 @@
         <v>38</v>
       </c>
       <c r="X13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y13" t="s">
         <v>38</v>
@@ -2052,13 +2052,13 @@
         <v>38</v>
       </c>
       <c r="AB13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC13" t="s">
         <v>39</v>
       </c>
       <c r="AD13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE13" t="s">
         <v>38</v>
@@ -2067,7 +2067,7 @@
         <v>39</v>
       </c>
       <c r="AG13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH13" t="s">
         <v>39</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
@@ -2090,13 +2090,13 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
         <v>39</v>
@@ -2108,13 +2108,13 @@
         <v>38</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" t="s">
         <v>38</v>
@@ -2126,19 +2126,19 @@
         <v>39</v>
       </c>
       <c r="Q14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R14" t="s">
         <v>39</v>
       </c>
       <c r="S14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V14" t="s">
         <v>39</v>
@@ -2147,7 +2147,7 @@
         <v>38</v>
       </c>
       <c r="X14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y14" t="s">
         <v>38</v>
@@ -2159,13 +2159,13 @@
         <v>38</v>
       </c>
       <c r="AB14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC14" t="s">
         <v>39</v>
       </c>
       <c r="AD14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE14" t="s">
         <v>38</v>
@@ -2174,7 +2174,7 @@
         <v>39</v>
       </c>
       <c r="AG14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH14" t="s">
         <v>39</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>67</v>
@@ -2197,13 +2197,13 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
         <v>39</v>
@@ -2215,13 +2215,13 @@
         <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N15" t="s">
         <v>38</v>
@@ -2233,19 +2233,19 @@
         <v>39</v>
       </c>
       <c r="Q15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R15" t="s">
         <v>39</v>
       </c>
       <c r="S15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V15" t="s">
         <v>39</v>
@@ -2254,7 +2254,7 @@
         <v>38</v>
       </c>
       <c r="X15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y15" t="s">
         <v>38</v>
@@ -2266,13 +2266,13 @@
         <v>38</v>
       </c>
       <c r="AB15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC15" t="s">
         <v>39</v>
       </c>
       <c r="AD15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE15" t="s">
         <v>38</v>
@@ -2281,7 +2281,7 @@
         <v>39</v>
       </c>
       <c r="AG15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH15" t="s">
         <v>39</v>
@@ -2304,19 +2304,19 @@
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s">
         <v>39</v>
@@ -2325,10 +2325,10 @@
         <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N16" t="s">
         <v>38</v>
@@ -2337,43 +2337,43 @@
         <v>38</v>
       </c>
       <c r="P16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q16" t="s">
         <v>39</v>
       </c>
       <c r="R16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S16" t="s">
         <v>39</v>
       </c>
       <c r="T16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W16" t="s">
         <v>38</v>
       </c>
       <c r="X16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z16" t="s">
         <v>39</v>
       </c>
       <c r="AA16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC16" t="s">
         <v>38</v>
@@ -2388,7 +2388,7 @@
         <v>38</v>
       </c>
       <c r="AG16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH16" t="s">
         <v>39</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -2411,7 +2411,7 @@
         <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -2423,7 +2423,7 @@
         <v>38</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J17" t="s">
         <v>39</v>
@@ -2432,31 +2432,31 @@
         <v>38</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M17" t="s">
         <v>38</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O17" t="s">
         <v>38</v>
       </c>
       <c r="P17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q17" t="s">
         <v>39</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S17" t="s">
         <v>39</v>
       </c>
       <c r="T17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U17" t="s">
         <v>38</v>
@@ -2474,16 +2474,16 @@
         <v>38</v>
       </c>
       <c r="Z17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD17" t="s">
         <v>38</v>
@@ -2492,21 +2492,21 @@
         <v>39</v>
       </c>
       <c r="AF17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH17" t="s">
         <v>39</v>
       </c>
       <c r="AI17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>74</v>
@@ -2515,52 +2515,52 @@
         <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
         <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J18" t="s">
         <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N18" t="s">
         <v>39</v>
       </c>
       <c r="O18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q18" t="s">
         <v>39</v>
       </c>
       <c r="R18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T18" t="s">
         <v>39</v>
@@ -2587,33 +2587,33 @@
         <v>39</v>
       </c>
       <c r="AB18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD18" t="s">
         <v>38</v>
       </c>
       <c r="AE18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF18" t="s">
         <v>38</v>
       </c>
       <c r="AG18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>76</v>
@@ -2622,7 +2622,7 @@
         <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>
@@ -2637,16 +2637,16 @@
         <v>38</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M19" t="s">
         <v>38</v>
@@ -2655,16 +2655,16 @@
         <v>39</v>
       </c>
       <c r="O19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q19" t="s">
         <v>39</v>
       </c>
       <c r="R19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S19" t="s">
         <v>39</v>
@@ -2673,16 +2673,16 @@
         <v>39</v>
       </c>
       <c r="U19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V19" t="s">
         <v>39</v>
       </c>
       <c r="W19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y19" t="s">
         <v>38</v>
@@ -2691,28 +2691,28 @@
         <v>38</v>
       </c>
       <c r="AA19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF19" t="s">
         <v>38</v>
       </c>
       <c r="AG19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI19" t="s">
         <v>38</v>
@@ -2729,22 +2729,22 @@
         <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J20" t="s">
         <v>39</v>
@@ -2753,13 +2753,13 @@
         <v>38</v>
       </c>
       <c r="L20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M20" t="s">
         <v>38</v>
       </c>
       <c r="N20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O20" t="s">
         <v>38</v>
@@ -2768,7 +2768,7 @@
         <v>38</v>
       </c>
       <c r="Q20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R20" t="s">
         <v>39</v>
@@ -2777,40 +2777,40 @@
         <v>38</v>
       </c>
       <c r="T20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V20" t="s">
         <v>38</v>
       </c>
       <c r="W20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB20" t="s">
         <v>39</v>
       </c>
       <c r="AC20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD20" t="s">
         <v>39</v>
       </c>
       <c r="AE20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF20" t="s">
         <v>39</v>
@@ -2819,7 +2819,7 @@
         <v>39</v>
       </c>
       <c r="AH20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI20" t="s">
         <v>38</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -2839,16 +2839,16 @@
         <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I21" t="s">
         <v>38</v>
@@ -2866,16 +2866,16 @@
         <v>38</v>
       </c>
       <c r="N21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R21" t="s">
         <v>39</v>
@@ -2884,13 +2884,13 @@
         <v>38</v>
       </c>
       <c r="T21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U21" t="s">
         <v>39</v>
       </c>
       <c r="V21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W21" t="s">
         <v>39</v>
@@ -2905,13 +2905,13 @@
         <v>38</v>
       </c>
       <c r="AA21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB21" t="s">
         <v>38</v>
       </c>
       <c r="AC21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD21" t="s">
         <v>39</v>
@@ -2920,21 +2920,21 @@
         <v>39</v>
       </c>
       <c r="AF21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH21" t="s">
         <v>38</v>
       </c>
       <c r="AI21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>83</v>
@@ -2943,7 +2943,7 @@
         <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
         <v>38</v>
@@ -2952,28 +2952,28 @@
         <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I22" t="s">
         <v>38</v>
       </c>
       <c r="J22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O22" t="s">
         <v>38</v>
@@ -2982,52 +2982,52 @@
         <v>38</v>
       </c>
       <c r="Q22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R22" t="s">
         <v>39</v>
       </c>
       <c r="S22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X22" t="s">
         <v>39</v>
       </c>
       <c r="Y22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z22" t="s">
         <v>38</v>
       </c>
       <c r="AA22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB22" t="s">
         <v>38</v>
       </c>
       <c r="AC22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG22" t="s">
         <v>39</v>
@@ -3036,12 +3036,12 @@
         <v>38</v>
       </c>
       <c r="AI22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
@@ -3050,37 +3050,37 @@
         <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
         <v>38</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K23" t="s">
         <v>38</v>
       </c>
       <c r="L23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O23" t="s">
         <v>38</v>
@@ -3089,16 +3089,16 @@
         <v>38</v>
       </c>
       <c r="Q23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S23" t="s">
         <v>38</v>
       </c>
       <c r="T23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U23" t="s">
         <v>38</v>
@@ -3110,37 +3110,37 @@
         <v>39</v>
       </c>
       <c r="X23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z23" t="s">
         <v>39</v>
       </c>
       <c r="AA23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB23" t="s">
         <v>39</v>
       </c>
       <c r="AC23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG23" t="s">
         <v>39</v>
       </c>
       <c r="AH23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI23" t="s">
         <v>38</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
@@ -3157,16 +3157,16 @@
         <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
         <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
@@ -3181,40 +3181,40 @@
         <v>38</v>
       </c>
       <c r="L24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M24" t="s">
         <v>38</v>
       </c>
       <c r="N24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P24" t="s">
         <v>38</v>
       </c>
       <c r="Q24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R24" t="s">
         <v>39</v>
       </c>
       <c r="S24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X24" t="s">
         <v>39</v>
@@ -3223,19 +3223,19 @@
         <v>39</v>
       </c>
       <c r="Z24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB24" t="s">
         <v>38</v>
       </c>
       <c r="AC24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE24" t="s">
         <v>38</v>
@@ -3250,12 +3250,12 @@
         <v>38</v>
       </c>
       <c r="AI24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -3264,16 +3264,16 @@
         <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" t="s">
         <v>39</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
@@ -3285,25 +3285,25 @@
         <v>39</v>
       </c>
       <c r="K25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M25" t="s">
         <v>38</v>
       </c>
       <c r="N25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P25" t="s">
         <v>38</v>
       </c>
       <c r="Q25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R25" t="s">
         <v>39</v>
@@ -3312,7 +3312,7 @@
         <v>38</v>
       </c>
       <c r="T25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U25" t="s">
         <v>39</v>
@@ -3327,34 +3327,34 @@
         <v>39</v>
       </c>
       <c r="Y25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD25" t="s">
         <v>38</v>
       </c>
       <c r="AE25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG25" t="s">
         <v>39</v>
       </c>
       <c r="AH25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI25" t="s">
         <v>38</v>
@@ -3371,28 +3371,28 @@
         <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
         <v>39</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
         <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I26" t="s">
         <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L26" t="s">
         <v>38</v>
@@ -3404,16 +3404,16 @@
         <v>39</v>
       </c>
       <c r="O26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P26" t="s">
         <v>38</v>
       </c>
       <c r="Q26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S26" t="s">
         <v>38</v>
@@ -3425,19 +3425,19 @@
         <v>38</v>
       </c>
       <c r="V26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X26" t="s">
         <v>39</v>
       </c>
       <c r="Y26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA26" t="s">
         <v>39</v>
@@ -3452,24 +3452,24 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF26" t="s">
         <v>38</v>
       </c>
       <c r="AG26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH26" t="s">
         <v>39</v>
       </c>
       <c r="AI26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
@@ -3484,16 +3484,16 @@
         <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
         <v>38</v>
       </c>
       <c r="H27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J27" t="s">
         <v>39</v>
@@ -3502,28 +3502,28 @@
         <v>39</v>
       </c>
       <c r="L27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N27" t="s">
         <v>39</v>
       </c>
       <c r="O27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q27" t="s">
         <v>38</v>
       </c>
       <c r="R27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T27" t="s">
         <v>39</v>
@@ -3532,22 +3532,22 @@
         <v>38</v>
       </c>
       <c r="V27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X27" t="s">
         <v>38</v>
       </c>
       <c r="Y27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB27" t="s">
         <v>39</v>
@@ -3556,27 +3556,27 @@
         <v>39</v>
       </c>
       <c r="AD27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF27" t="s">
         <v>38</v>
       </c>
       <c r="AG27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH27" t="s">
         <v>39</v>
       </c>
       <c r="AI27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
         <v>96</v>
@@ -3591,13 +3591,13 @@
         <v>39</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
         <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I28" t="s">
         <v>39</v>
@@ -3606,7 +3606,7 @@
         <v>39</v>
       </c>
       <c r="K28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L28" t="s">
         <v>38</v>
@@ -3615,40 +3615,40 @@
         <v>39</v>
       </c>
       <c r="N28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O28" t="s">
         <v>38</v>
       </c>
       <c r="P28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R28" t="s">
         <v>39</v>
       </c>
       <c r="S28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U28" t="s">
         <v>38</v>
       </c>
       <c r="V28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z28" t="s">
         <v>38</v>
@@ -3663,22 +3663,22 @@
         <v>38</v>
       </c>
       <c r="AD28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF28" t="s">
         <v>38</v>
       </c>
       <c r="AG28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH28" t="s">
         <v>39</v>
       </c>
       <c r="AI28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
@@ -3698,7 +3698,7 @@
         <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G29" t="s">
         <v>38</v>
@@ -3719,40 +3719,40 @@
         <v>39</v>
       </c>
       <c r="M29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R29" t="s">
         <v>38</v>
       </c>
       <c r="S29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T29" t="s">
         <v>39</v>
       </c>
       <c r="U29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W29" t="s">
         <v>38</v>
       </c>
       <c r="X29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y29" t="s">
         <v>38</v>
@@ -3761,13 +3761,13 @@
         <v>39</v>
       </c>
       <c r="AA29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD29" t="s">
         <v>38</v>
@@ -3776,13 +3776,13 @@
         <v>39</v>
       </c>
       <c r="AF29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG29" t="s">
         <v>39</v>
       </c>
       <c r="AH29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI29" t="s">
         <v>39</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
         <v>101</v>
@@ -3808,7 +3808,7 @@
         <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -3817,7 +3817,7 @@
         <v>38</v>
       </c>
       <c r="J30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K30" t="s">
         <v>39</v>
@@ -3829,10 +3829,10 @@
         <v>38</v>
       </c>
       <c r="N30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P30" t="s">
         <v>39</v>
@@ -3841,7 +3841,7 @@
         <v>39</v>
       </c>
       <c r="R30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S30" t="s">
         <v>38</v>
@@ -3856,25 +3856,25 @@
         <v>39</v>
       </c>
       <c r="W30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB30" t="s">
         <v>38</v>
       </c>
       <c r="AC30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD30" t="s">
         <v>38</v>
@@ -3883,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="AF30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG30" t="s">
         <v>39</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>103</v>
@@ -3915,7 +3915,7 @@
         <v>39</v>
       </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H31" t="s">
         <v>39</v>
@@ -3924,7 +3924,7 @@
         <v>38</v>
       </c>
       <c r="J31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K31" t="s">
         <v>39</v>
@@ -3936,10 +3936,10 @@
         <v>38</v>
       </c>
       <c r="N31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P31" t="s">
         <v>39</v>
@@ -3948,13 +3948,13 @@
         <v>39</v>
       </c>
       <c r="R31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S31" t="s">
         <v>38</v>
       </c>
       <c r="T31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U31" t="s">
         <v>38</v>
@@ -3963,25 +3963,25 @@
         <v>39</v>
       </c>
       <c r="W31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB31" t="s">
         <v>38</v>
       </c>
       <c r="AC31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD31" t="s">
         <v>38</v>
@@ -3990,7 +3990,7 @@
         <v>39</v>
       </c>
       <c r="AF31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG31" t="s">
         <v>39</v>
@@ -3999,7 +3999,7 @@
         <v>39</v>
       </c>
       <c r="AI31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
@@ -4013,10 +4013,10 @@
         <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
         <v>38</v>
@@ -4025,19 +4025,19 @@
         <v>39</v>
       </c>
       <c r="H32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I32" t="s">
         <v>38</v>
       </c>
       <c r="J32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K32" t="s">
         <v>38</v>
       </c>
       <c r="L32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M32" t="s">
         <v>39</v>
@@ -4049,22 +4049,22 @@
         <v>39</v>
       </c>
       <c r="P32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V32" t="s">
         <v>39</v>
@@ -4076,7 +4076,7 @@
         <v>39</v>
       </c>
       <c r="Y32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z32" t="s">
         <v>39</v>
@@ -4088,10 +4088,10 @@
         <v>39</v>
       </c>
       <c r="AC32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE32" t="s">
         <v>38</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>108</v>
@@ -4120,10 +4120,10 @@
         <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
         <v>38</v>
@@ -4141,19 +4141,19 @@
         <v>38</v>
       </c>
       <c r="K33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N33" t="s">
         <v>39</v>
       </c>
       <c r="O33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P33" t="s">
         <v>39</v>
@@ -4168,7 +4168,7 @@
         <v>39</v>
       </c>
       <c r="T33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U33" t="s">
         <v>38</v>
@@ -4177,16 +4177,16 @@
         <v>39</v>
       </c>
       <c r="W33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA33" t="s">
         <v>39</v>
@@ -4198,13 +4198,13 @@
         <v>38</v>
       </c>
       <c r="AD33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AE33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG33" t="s">
         <v>38</v>
@@ -4213,12 +4213,12 @@
         <v>38</v>
       </c>
       <c r="AI33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
@@ -4230,10 +4230,10 @@
         <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
@@ -4242,22 +4242,22 @@
         <v>39</v>
       </c>
       <c r="I34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J34" t="s">
         <v>38</v>
       </c>
       <c r="K34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M34" t="s">
         <v>39</v>
       </c>
       <c r="N34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O34" t="s">
         <v>39</v>
@@ -4266,13 +4266,13 @@
         <v>38</v>
       </c>
       <c r="Q34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T34" t="s">
         <v>39</v>
@@ -4290,22 +4290,22 @@
         <v>39</v>
       </c>
       <c r="Y34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA34" t="s">
         <v>39</v>
       </c>
       <c r="AB34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC34" t="s">
         <v>39</v>
       </c>
       <c r="AD34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE34" t="s">
         <v>39</v>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>112</v>
@@ -4334,10 +4334,10 @@
         <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
         <v>38</v>
@@ -4346,19 +4346,19 @@
         <v>39</v>
       </c>
       <c r="H35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J35" t="s">
         <v>38</v>
       </c>
       <c r="K35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M35" t="s">
         <v>39</v>
@@ -4367,13 +4367,13 @@
         <v>38</v>
       </c>
       <c r="O35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R35" t="s">
         <v>39</v>
@@ -4388,46 +4388,46 @@
         <v>38</v>
       </c>
       <c r="V35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W35" t="s">
         <v>39</v>
       </c>
       <c r="X35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z35" t="s">
         <v>38</v>
       </c>
       <c r="AA35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB35" t="s">
         <v>39</v>
       </c>
       <c r="AC35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD35" t="s">
         <v>38</v>
       </c>
       <c r="AE35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH35" t="s">
         <v>38</v>
       </c>
       <c r="AI35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>